<commit_message>
SLLC for PUFS 2.0
</commit_message>
<xml_diff>
--- a/Organization/Kopie von Arbeitszeitplan .xlsx
+++ b/Organization/Kopie von Arbeitszeitplan .xlsx
@@ -206,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -232,15 +232,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -259,6 +250,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -541,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,15 +586,15 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21"/>
+      <c r="H3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="27"/>
       <c r="O3" t="s">
         <v>5</v>
       </c>
@@ -690,15 +691,15 @@
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="24"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="21"/>
       <c r="O7" t="s">
         <v>5</v>
       </c>
@@ -723,15 +724,15 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="27"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="24"/>
       <c r="O8" t="s">
         <v>5</v>
       </c>
@@ -740,22 +741,31 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
+      <c r="A9" s="7">
+        <v>42964</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666663</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="18"/>
+      <c r="H9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="24"/>
       <c r="O9" t="s">
         <v>5</v>
       </c>
@@ -1923,13 +1933,18 @@
       <c r="A48" t="s">
         <v>6</v>
       </c>
-      <c r="E48">
-        <f>SUM(E3:E9)</f>
-        <v>0.35416666666666663</v>
+      <c r="E48" s="28">
+        <f>SUM(E7:E9)</f>
+        <v>0.45833333333333326</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="H5:N5"/>
+    <mergeCell ref="H4:N4"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="H13:N13"/>
     <mergeCell ref="H14:N14"/>
     <mergeCell ref="H7:N7"/>
     <mergeCell ref="H8:N8"/>
@@ -1937,11 +1952,6 @@
     <mergeCell ref="H10:N10"/>
     <mergeCell ref="H11:N11"/>
     <mergeCell ref="H12:N12"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="H5:N5"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="H13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Start programming euclidean geometry, LDCP codes
</commit_message>
<xml_diff>
--- a/Organization/Kopie von Arbeitszeitplan .xlsx
+++ b/Organization/Kopie von Arbeitszeitplan .xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="11">
   <si>
     <t>Datum</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>LDPC-codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDPC-codes construction, Start Programming euclidian geometry </t>
   </si>
 </sst>
 </file>
@@ -209,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -263,6 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -546,7 +550,7 @@
   <dimension ref="A2:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H14" sqref="H14:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +726,7 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="8">
-        <f t="shared" ref="E8:E12" si="0">C8-B8</f>
+        <f t="shared" ref="E8:E14" si="0">C8-B8</f>
         <v>0.16666666666666669</v>
       </c>
       <c r="F8" s="5"/>
@@ -879,21 +883,28 @@
       <c r="A13" s="7">
         <v>42967</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="8">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.5</v>
+      </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="19"/>
+      <c r="H13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="25"/>
       <c r="O13" t="s">
         <v>5</v>
       </c>
@@ -905,21 +916,28 @@
       <c r="A14" s="7">
         <v>42968</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="29">
+        <v>0.625</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.875</v>
+      </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="19"/>
+      <c r="H14" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="25"/>
       <c r="O14" t="s">
         <v>5</v>
       </c>
@@ -1985,7 +2003,7 @@
       </c>
       <c r="E48" s="16">
         <f>SUM(E7:E47)</f>
-        <v>0.77083333333333326</v>
+        <v>1.1041666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>